<commit_message>
Add unique constraint to materialSampleID and edit test data accordingly
</commit_message>
<xml_diff>
--- a/scripts/import-test/input/jane.doe@univ.se_210902-212121_ampliseq.xlsx
+++ b/scripts/import-test/input/jane.doe@univ.se_210902-212121_ampliseq.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/molmod/static/downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/scripts/import-test/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FA3F2F-DBE6-9B46-8AD4-A6936F4EDDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FAE807-D361-F443-8C8D-56A01DE1F771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7360" yWindow="9760" windowWidth="38000" windowHeight="14600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7360" yWindow="9760" windowWidth="38000" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="307">
   <si>
     <t>event_id_alias</t>
   </si>
@@ -752,12 +752,6 @@
     <t>Anna Andersson|Björn Bengtsson</t>
   </si>
   <si>
-    <t>SAMEA3724535</t>
-  </si>
-  <si>
-    <t>SAMEA3724536</t>
-  </si>
-  <si>
     <t>Field header: 'temperature (°C)', value: '16.9'</t>
   </si>
   <si>
@@ -960,6 +954,15 @@
   </si>
   <si>
     <t>emof-simple (a simplified version of emof, used by ASV portal only)</t>
+  </si>
+  <si>
+    <t>SOMENO3724531</t>
+  </si>
+  <si>
+    <t>SOMENO3724532</t>
+  </si>
+  <si>
+    <t>SOMENO3724533</t>
   </si>
 </sst>
 </file>
@@ -1703,8 +1706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD991"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1789,7 +1792,7 @@
         <v>199</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>222</v>
+        <v>304</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>202</v>
@@ -1824,7 +1827,7 @@
         <v>198</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>236</v>
+        <v>305</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>201</v>
@@ -1870,7 +1873,7 @@
         <v>197</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>237</v>
+        <v>306</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>200</v>
@@ -5257,7 +5260,7 @@
         <v>21</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>22</v>
@@ -5272,7 +5275,7 @@
         <v>25</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>26</v>
@@ -5298,7 +5301,7 @@
         <v>29</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>207</v>
@@ -5313,7 +5316,7 @@
         <v>123</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>211</v>
@@ -5339,7 +5342,7 @@
         <v>29</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>207</v>
@@ -5354,7 +5357,7 @@
         <v>123</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>211</v>
@@ -5380,7 +5383,7 @@
         <v>29</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>207</v>
@@ -5395,7 +5398,7 @@
         <v>123</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>211</v>
@@ -12760,28 +12763,28 @@
     </row>
     <row r="2" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>250</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="M2" s="5">
         <v>2235</v>
@@ -12795,28 +12798,28 @@
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>255</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>257</v>
       </c>
       <c r="M3" s="5">
         <v>1033</v>
@@ -12830,22 +12833,22 @@
     </row>
     <row r="4" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>249</v>
       </c>
       <c r="M4" s="5">
         <v>795</v>
@@ -12859,28 +12862,28 @@
     </row>
     <row r="5" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>266</v>
       </c>
       <c r="M5" s="5">
         <v>134</v>
@@ -12894,28 +12897,28 @@
     </row>
     <row r="6" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>267</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>269</v>
       </c>
       <c r="M6" s="5">
         <v>572</v>
@@ -12929,28 +12932,28 @@
     </row>
     <row r="7" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>266</v>
       </c>
       <c r="M7" s="5">
         <v>47</v>
@@ -12964,31 +12967,31 @@
     </row>
     <row r="8" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>278</v>
       </c>
       <c r="M8" s="5">
         <v>40</v>
@@ -13002,28 +13005,28 @@
     </row>
     <row r="9" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>279</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>281</v>
       </c>
       <c r="M9" s="5">
         <v>99</v>
@@ -13037,25 +13040,25 @@
     </row>
     <row r="10" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>256</v>
       </c>
       <c r="M10" s="5">
         <v>312</v>
@@ -13069,28 +13072,28 @@
     </row>
     <row r="11" spans="1:15" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>286</v>
       </c>
       <c r="M11" s="5">
         <v>147</v>
@@ -13580,7 +13583,7 @@
   </sheetPr>
   <dimension ref="A1:AA1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
@@ -13647,7 +13650,7 @@
     </row>
     <row r="2" spans="1:27" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="54" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>0</v>
@@ -13665,7 +13668,7 @@
         <v>63</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H2" s="35" t="s">
         <v>199</v>
@@ -13796,7 +13799,7 @@
         <v>70</v>
       </c>
       <c r="G5" s="47" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H5" s="42"/>
       <c r="I5" s="19"/>
@@ -13837,7 +13840,7 @@
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="44" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H6" s="36">
         <v>80698</v>
@@ -13880,7 +13883,7 @@
         <v>75</v>
       </c>
       <c r="G7" s="44" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H7" s="37" t="s">
         <v>76</v>
@@ -14087,7 +14090,7 @@
         <v>91</v>
       </c>
       <c r="G12" s="44" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H12" s="36" t="s">
         <v>235</v>
@@ -14391,7 +14394,7 @@
     </row>
     <row r="20" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="54" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B20" s="23" t="s">
         <v>0</v>
@@ -14409,7 +14412,7 @@
         <v>63</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H20" s="35" t="s">
         <v>199</v>
@@ -14436,7 +14439,7 @@
     </row>
     <row r="21" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A21" s="54" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B21" s="23" t="s">
         <v>18</v>
@@ -14477,7 +14480,7 @@
     </row>
     <row r="22" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="54" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B22" s="23" t="s">
         <v>19</v>
@@ -14516,7 +14519,7 @@
     </row>
     <row r="23" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="54" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B23" s="23" t="s">
         <v>20</v>
@@ -14555,7 +14558,7 @@
     </row>
     <row r="24" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="54" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B24" s="23" t="s">
         <v>21</v>
@@ -14594,20 +14597,20 @@
     </row>
     <row r="25" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="54" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B25" s="48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C25" s="48" t="s">
         <v>62</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="53" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G25" s="25"/>
       <c r="H25" s="36"/>
@@ -14633,7 +14636,7 @@
     </row>
     <row r="26" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="54" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B26" s="23" t="s">
         <v>22</v>
@@ -14672,7 +14675,7 @@
     </row>
     <row r="27" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="54" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B27" s="23" t="s">
         <v>23</v>
@@ -14711,7 +14714,7 @@
     </row>
     <row r="28" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="54" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B28" s="23" t="s">
         <v>24</v>
@@ -14750,7 +14753,7 @@
     </row>
     <row r="29" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="54" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B29" s="23" t="s">
         <v>25</v>
@@ -14789,10 +14792,10 @@
     </row>
     <row r="30" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="54" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B30" s="50" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C30" s="23" t="s">
         <v>62</v>
@@ -14807,10 +14810,10 @@
         <v>63</v>
       </c>
       <c r="G30" s="51" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H30" s="52" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
@@ -14834,7 +14837,7 @@
     </row>
     <row r="31" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A31" s="54" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B31" s="23" t="s">
         <v>26</v>
@@ -14852,7 +14855,7 @@
         <v>227</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H31" s="36" t="s">
         <v>228</v>
@@ -14879,7 +14882,7 @@
     </row>
     <row r="32" spans="1:27" ht="204" x14ac:dyDescent="0.2">
       <c r="A32" s="54" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B32" s="23" t="s">
         <v>27</v>
@@ -14897,7 +14900,7 @@
         <v>232</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H32" s="36" t="s">
         <v>233</v>
@@ -14924,7 +14927,7 @@
     </row>
     <row r="33" spans="1:27" ht="154" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="57" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>28</v>
@@ -14942,7 +14945,7 @@
         <v>126</v>
       </c>
       <c r="G33" s="29" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H33" s="38" t="s">
         <v>234</v>
@@ -14969,7 +14972,7 @@
     </row>
     <row r="34" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="54" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>0</v>
@@ -14987,7 +14990,7 @@
         <v>63</v>
       </c>
       <c r="G34" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H34" s="35" t="s">
         <v>199</v>
@@ -15032,7 +15035,7 @@
         <v>130</v>
       </c>
       <c r="G35" s="44" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H35" s="36"/>
       <c r="I35" s="19"/>
@@ -15465,7 +15468,7 @@
     </row>
     <row r="46" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A46" s="61" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B46" s="20" t="s">
         <v>0</v>
@@ -15483,7 +15486,7 @@
         <v>63</v>
       </c>
       <c r="G46" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H46" s="35" t="s">
         <v>199</v>
@@ -15528,10 +15531,10 @@
         <v>63</v>
       </c>
       <c r="G47" s="45" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H47" s="38" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I47" s="19"/>
       <c r="J47" s="19"/>
@@ -15555,7 +15558,7 @@
     </row>
     <row r="48" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A48" s="54" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>161</v>
@@ -15618,7 +15621,7 @@
         <v>63</v>
       </c>
       <c r="G49" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H49" s="35" t="s">
         <v>199</v>
@@ -15790,7 +15793,7 @@
         <v>177</v>
       </c>
       <c r="G53" s="43" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H53" s="36"/>
       <c r="I53" s="19"/>

</xml_diff>